<commit_message>
ng: oncho update forms
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2023/june/ng_oncho_bsc_202306_1_capture.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2023/june/ng_oncho_bsc_202306_1_capture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2023\june\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCA1A73-F3C1-4701-9EBA-39C60ACCF247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9309E28-63ED-4063-88B4-9F21DA926BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="145">
   <si>
     <t>type</t>
   </si>
@@ -305,144 +305,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>GOMBE</t>
-  </si>
-  <si>
-    <t>AKKO</t>
-  </si>
-  <si>
-    <t>BALANGA</t>
-  </si>
-  <si>
-    <t>BILLIRI</t>
-  </si>
-  <si>
-    <t>DUKKU</t>
-  </si>
-  <si>
-    <t>NAFADA</t>
-  </si>
-  <si>
-    <t>FUNAKAYE</t>
-  </si>
-  <si>
-    <t>SHOMGOM</t>
-  </si>
-  <si>
-    <t>KALTUNGO</t>
-  </si>
-  <si>
-    <t>KWAMI</t>
-  </si>
-  <si>
-    <t>YAMALTU/DEBA</t>
-  </si>
-  <si>
-    <t>KOMBANI</t>
-  </si>
-  <si>
-    <t>KUMO</t>
-  </si>
-  <si>
-    <t>WURO DOLE</t>
-  </si>
-  <si>
-    <t>BANGU</t>
-  </si>
-  <si>
-    <t>CHUM</t>
-  </si>
-  <si>
-    <t>DADIYA</t>
-  </si>
-  <si>
-    <t>GALENGU</t>
-  </si>
-  <si>
-    <t>KULKUL</t>
-  </si>
-  <si>
-    <t>DOKORO</t>
-  </si>
-  <si>
-    <t>GARIN BULAMO</t>
-  </si>
-  <si>
-    <t>BANA</t>
-  </si>
-  <si>
-    <t>WAKALU</t>
-  </si>
-  <si>
-    <t>WURO BONGO</t>
-  </si>
-  <si>
-    <t>MAMUDA</t>
-  </si>
-  <si>
-    <t>MALARI</t>
-  </si>
-  <si>
-    <t>POPANDI</t>
-  </si>
-  <si>
-    <t>TULA WANGE</t>
-  </si>
-  <si>
-    <t>BULTURI</t>
-  </si>
-  <si>
-    <t>GUDOKO</t>
-  </si>
-  <si>
-    <t>JIGAWA</t>
-  </si>
-  <si>
-    <t>JIGAWA KUKA</t>
-  </si>
-  <si>
-    <t>MADA</t>
-  </si>
-  <si>
-    <t>DWAJA</t>
-  </si>
-  <si>
-    <t>HINNA</t>
-  </si>
-  <si>
-    <t>CHONGWOM</t>
-  </si>
-  <si>
-    <t>ng_oncho_bsc_202306_1_capture</t>
-  </si>
-  <si>
-    <t>(2023 June) - 1. Human Landing Catches</t>
-  </si>
-  <si>
-    <t>BANGU (AKKO)</t>
-  </si>
-  <si>
-    <t>GARKO</t>
-  </si>
-  <si>
-    <t>KULANI / DEGRE /SIKKAM</t>
-  </si>
-  <si>
-    <t>MWONA</t>
-  </si>
-  <si>
-    <t>BILLIRI SOUTH</t>
-  </si>
-  <si>
-    <t>TAL</t>
-  </si>
-  <si>
-    <t>GWANI / SHINGA / WADE</t>
-  </si>
-  <si>
-    <t>JAGALI NORTH</t>
-  </si>
-  <si>
     <t>LGA</t>
   </si>
   <si>
@@ -480,6 +342,132 @@
   </si>
   <si>
     <t>select_one m_t</t>
+  </si>
+  <si>
+    <t>CROSS RIVER</t>
+  </si>
+  <si>
+    <t>AKAMKPA</t>
+  </si>
+  <si>
+    <t>BEKWARRA</t>
+  </si>
+  <si>
+    <t>BIASE</t>
+  </si>
+  <si>
+    <t>BOKI</t>
+  </si>
+  <si>
+    <t>ETUNG</t>
+  </si>
+  <si>
+    <t>IKOM</t>
+  </si>
+  <si>
+    <t>OBANLIKU</t>
+  </si>
+  <si>
+    <t>OBIANLIKU</t>
+  </si>
+  <si>
+    <t>OBUBRA</t>
+  </si>
+  <si>
+    <t>OBUDU</t>
+  </si>
+  <si>
+    <t>YAKURR</t>
+  </si>
+  <si>
+    <t>YALA</t>
+  </si>
+  <si>
+    <t>AKING</t>
+  </si>
+  <si>
+    <t>AKWA IBAMI</t>
+  </si>
+  <si>
+    <t>EKANG</t>
+  </si>
+  <si>
+    <t>EKONG</t>
+  </si>
+  <si>
+    <t>MFAMOSING</t>
+  </si>
+  <si>
+    <t>OBAN</t>
+  </si>
+  <si>
+    <t>AFRIKE</t>
+  </si>
+  <si>
+    <t>AKPARAVUNI</t>
+  </si>
+  <si>
+    <t>BANSAN</t>
+  </si>
+  <si>
+    <t>DANARE</t>
+  </si>
+  <si>
+    <t>OKWA</t>
+  </si>
+  <si>
+    <t>ABIA</t>
+  </si>
+  <si>
+    <t>EKURI EYENGYEG</t>
+  </si>
+  <si>
+    <t>ETARA</t>
+  </si>
+  <si>
+    <t>ABARAGBA</t>
+  </si>
+  <si>
+    <t>BASSINGE</t>
+  </si>
+  <si>
+    <t>BAYALUGA</t>
+  </si>
+  <si>
+    <t>BUANCHOR</t>
+  </si>
+  <si>
+    <t>KIGOL</t>
+  </si>
+  <si>
+    <t>OLD IKWETE</t>
+  </si>
+  <si>
+    <t>EDONDON</t>
+  </si>
+  <si>
+    <t>BEBI</t>
+  </si>
+  <si>
+    <t>AGOI IBAMI</t>
+  </si>
+  <si>
+    <t>OTUKPO</t>
+  </si>
+  <si>
+    <t>site_id</t>
+  </si>
+  <si>
+    <t>select_one site_id</t>
+  </si>
+  <si>
+    <t>community = ${s_community}</t>
+  </si>
+  <si>
+    <t>(2023 June) - 1. Human Landing Catches V2.1</t>
+  </si>
+  <si>
+    <t>ng_oncho_bsc_202306_1_capture_v2_1</t>
   </si>
 </sst>
 </file>
@@ -499,7 +487,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -507,14 +495,14 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -522,7 +510,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -588,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -640,6 +628,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -925,10 +914,10 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD19"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1017,7 +1006,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="9"/>
@@ -1037,7 +1026,7 @@
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="20" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -1059,13 +1048,13 @@
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1">
       <c r="A5" s="22" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>22</v>
@@ -1082,8 +1071,8 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="A6" s="9" t="s">
-        <v>24</v>
+      <c r="A6" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>26</v>
@@ -1101,7 +1090,9 @@
         <v>16</v>
       </c>
       <c r="K6" s="6"/>
-      <c r="L6" s="9"/>
+      <c r="L6" s="22" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1">
       <c r="A7" s="9" t="s">
@@ -1150,13 +1141,13 @@
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>34</v>
@@ -1433,11 +1424,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD12"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1662,46 +1653,46 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="19" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="19" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="19" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="19" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1709,10 +1700,10 @@
         <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1720,13 +1711,13 @@
         <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1734,13 +1725,13 @@
         <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1748,13 +1739,13 @@
         <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1762,13 +1753,13 @@
         <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1776,13 +1767,13 @@
         <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1790,13 +1781,13 @@
         <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1804,13 +1795,13 @@
         <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1818,13 +1809,13 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1832,13 +1823,13 @@
         <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1846,55 +1837,58 @@
         <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>90</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
-      </c>
-      <c r="E39" t="s">
-        <v>91</v>
+        <v>115</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" t="s">
-        <v>128</v>
-      </c>
-      <c r="E40" t="s">
-        <v>91</v>
-      </c>
+      <c r="D40" s="23"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1902,13 +1896,13 @@
         <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="E42" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1916,13 +1910,13 @@
         <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="E43" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1930,13 +1924,13 @@
         <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="E44" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1944,13 +1938,13 @@
         <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="E45" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1958,13 +1952,13 @@
         <v>67</v>
       </c>
       <c r="B46" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" t="s">
+        <v>121</v>
+      </c>
+      <c r="E46" t="s">
         <v>104</v>
-      </c>
-      <c r="C46" t="s">
-        <v>104</v>
-      </c>
-      <c r="E46" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1972,13 +1966,13 @@
         <v>67</v>
       </c>
       <c r="B47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" t="s">
         <v>105</v>
-      </c>
-      <c r="C47" t="s">
-        <v>105</v>
-      </c>
-      <c r="E47" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1986,13 +1980,13 @@
         <v>67</v>
       </c>
       <c r="B48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" t="s">
         <v>106</v>
-      </c>
-      <c r="C48" t="s">
-        <v>106</v>
-      </c>
-      <c r="E48" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2000,13 +1994,13 @@
         <v>67</v>
       </c>
       <c r="B49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" t="s">
+        <v>124</v>
+      </c>
+      <c r="E49" t="s">
         <v>107</v>
-      </c>
-      <c r="C49" t="s">
-        <v>107</v>
-      </c>
-      <c r="E49" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2014,13 +2008,13 @@
         <v>67</v>
       </c>
       <c r="B50" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C50" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E50" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2028,13 +2022,13 @@
         <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E51" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2042,13 +2036,13 @@
         <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C52" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E52" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2056,13 +2050,13 @@
         <v>67</v>
       </c>
       <c r="B53" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53" t="s">
         <v>108</v>
-      </c>
-      <c r="C53" t="s">
-        <v>108</v>
-      </c>
-      <c r="E53" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2070,13 +2064,13 @@
         <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E54" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2084,13 +2078,13 @@
         <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="C55" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="E55" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2098,13 +2092,13 @@
         <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="C56" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="E56" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2112,13 +2106,13 @@
         <v>67</v>
       </c>
       <c r="B57" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" t="s">
+        <v>132</v>
+      </c>
+      <c r="E57" t="s">
         <v>110</v>
-      </c>
-      <c r="C57" t="s">
-        <v>110</v>
-      </c>
-      <c r="E57" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2126,13 +2120,13 @@
         <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="E58" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2140,13 +2134,13 @@
         <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="E59" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2154,13 +2148,13 @@
         <v>67</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="E60" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2168,13 +2162,13 @@
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="C61" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="E61" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2182,13 +2176,13 @@
         <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="C62" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="E62" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2196,13 +2190,13 @@
         <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="C63" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="E63" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2210,158 +2204,354 @@
         <v>67</v>
       </c>
       <c r="B64" t="s">
+        <v>139</v>
+      </c>
+      <c r="C64" t="s">
+        <v>139</v>
+      </c>
+      <c r="E64" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B66">
+        <v>101</v>
+      </c>
+      <c r="C66">
+        <v>101</v>
+      </c>
+      <c r="F66" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B67">
+        <v>102</v>
+      </c>
+      <c r="C67">
+        <v>102</v>
+      </c>
+      <c r="F67" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B68">
+        <v>103</v>
+      </c>
+      <c r="C68">
+        <v>103</v>
+      </c>
+      <c r="F68" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69">
+        <v>104</v>
+      </c>
+      <c r="C69">
+        <v>104</v>
+      </c>
+      <c r="F69" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70">
+        <v>105</v>
+      </c>
+      <c r="C70">
+        <v>105</v>
+      </c>
+      <c r="F70" t="s">
         <v>120</v>
       </c>
-      <c r="C64" t="s">
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71">
+        <v>106</v>
+      </c>
+      <c r="C71">
+        <v>106</v>
+      </c>
+      <c r="F71" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72">
+        <v>107</v>
+      </c>
+      <c r="C72">
+        <v>107</v>
+      </c>
+      <c r="F72" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73">
+        <v>108</v>
+      </c>
+      <c r="C73">
+        <v>108</v>
+      </c>
+      <c r="F73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74">
+        <v>109</v>
+      </c>
+      <c r="C74">
+        <v>109</v>
+      </c>
+      <c r="F74" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B75">
+        <v>110</v>
+      </c>
+      <c r="C75">
+        <v>110</v>
+      </c>
+      <c r="F75" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76">
+        <v>111</v>
+      </c>
+      <c r="C76">
+        <v>111</v>
+      </c>
+      <c r="F76" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77">
+        <v>112</v>
+      </c>
+      <c r="C77">
+        <v>112</v>
+      </c>
+      <c r="F77" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B78">
+        <v>113</v>
+      </c>
+      <c r="C78">
+        <v>113</v>
+      </c>
+      <c r="F78" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B79">
+        <v>114</v>
+      </c>
+      <c r="C79">
+        <v>114</v>
+      </c>
+      <c r="F79" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B80">
+        <v>115</v>
+      </c>
+      <c r="C80">
+        <v>115</v>
+      </c>
+      <c r="F80" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B81">
+        <v>116</v>
+      </c>
+      <c r="C81">
+        <v>116</v>
+      </c>
+      <c r="F81" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B82">
+        <v>117</v>
+      </c>
+      <c r="C82">
+        <v>117</v>
+      </c>
+      <c r="F82" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83">
+        <v>118</v>
+      </c>
+      <c r="C83">
+        <v>118</v>
+      </c>
+      <c r="F83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84">
+        <v>119</v>
+      </c>
+      <c r="C84">
+        <v>119</v>
+      </c>
+      <c r="F84" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B85">
         <v>120</v>
       </c>
-      <c r="E64" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" t="s">
-        <v>67</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C85">
+        <v>120</v>
+      </c>
+      <c r="F85" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B86">
         <v>121</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C86">
         <v>121</v>
       </c>
-      <c r="E65" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
-        <v>67</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="F86" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B87">
         <v>122</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C87">
         <v>122</v>
       </c>
-      <c r="E66" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67" t="s">
-        <v>114</v>
-      </c>
-      <c r="C67" t="s">
-        <v>114</v>
-      </c>
-      <c r="E67" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" t="s">
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>95</v>
-      </c>
-      <c r="C68" t="s">
-        <v>95</v>
-      </c>
-      <c r="E68" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" t="s">
-        <v>67</v>
-      </c>
-      <c r="B69" t="s">
-        <v>125</v>
-      </c>
-      <c r="C69" t="s">
-        <v>125</v>
-      </c>
-      <c r="E69" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" t="s">
-        <v>67</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="F87" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B88">
         <v>123</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C88">
         <v>123</v>
       </c>
-      <c r="E70" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" t="s">
-        <v>116</v>
-      </c>
-      <c r="C71" t="s">
-        <v>116</v>
-      </c>
-      <c r="E71" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" t="s">
-        <v>67</v>
-      </c>
-      <c r="B72" t="s">
-        <v>134</v>
-      </c>
-      <c r="C72" t="s">
-        <v>134</v>
-      </c>
-      <c r="E72" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" t="s">
-        <v>67</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="F88" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89">
         <v>124</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C89">
         <v>124</v>
       </c>
-      <c r="E73" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" t="s">
-        <v>67</v>
-      </c>
-      <c r="B74" t="s">
-        <v>135</v>
-      </c>
-      <c r="C74" t="s">
-        <v>135</v>
-      </c>
-      <c r="E74" t="s">
-        <v>100</v>
+      <c r="F89" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A51:B96">
-    <sortCondition ref="B51:B96"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:B86">
+    <sortCondition ref="B53:B86"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2372,8 +2562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2395,10 +2585,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" t="s">
-        <v>126</v>
+        <v>143</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>144</v>
       </c>
       <c r="C2" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
ng: add oncho entomo forms
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2023/june/ng_oncho_bsc_202306_1_capture.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2023/june/ng_oncho_bsc_202306_1_capture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2023\june\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9309E28-63ED-4063-88B4-9F21DA926BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235B66C2-6515-489E-99B3-C27377166C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -464,10 +464,10 @@
     <t>community = ${s_community}</t>
   </si>
   <si>
-    <t>(2023 June) - 1. Human Landing Catches V2.1</t>
-  </si>
-  <si>
     <t>ng_oncho_bsc_202306_1_capture_v2_1</t>
+  </si>
+  <si>
+    <t>(2023 June) - 5. Human Landing Catches V2.1</t>
   </si>
 </sst>
 </file>
@@ -1426,9 +1426,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2562,8 +2562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2585,10 +2585,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>143</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>144</v>
       </c>
       <c r="C2" t="s">
         <v>89</v>

</xml_diff>